<commit_message>
Integration of the integration of excel
changed the excel load and write of some of the functions
loadDesign
-changed the streams to just use one raw file
-designation now done outside of the loop throught the units
--used a lookup struct

xlsReadPretty
- option tags to do postprocessing functions
- fixed off by one error on the left col

EHSexe
- do all the write calls in one call with new writew function

Classdesignations.xlsx
- now has everything on the same sheet and with same row names
</commit_message>
<xml_diff>
--- a/GlobalVars/classdesignations.xlsx
+++ b/GlobalVars/classdesignations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="17235" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="17235" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -414,147 +414,195 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F12"/>
+  <dimension ref="A2:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="C3">
+        <f>67*10^-6</f>
+        <v>6.7000000000000002E-5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3">
         <v>2</v>
       </c>
-      <c r="D3">
+      <c r="F3">
         <v>1</v>
       </c>
-      <c r="E3">
+      <c r="G3">
         <v>3</v>
       </c>
-      <c r="F3">
+      <c r="H3">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="C4">
+        <f>6.7*10^-6</f>
+        <v>6.7000000000000002E-6</v>
+      </c>
+      <c r="E4">
         <v>1</v>
       </c>
-      <c r="D4">
+      <c r="F4">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="C5">
+        <f>67*10^-6</f>
+        <v>6.7000000000000002E-5</v>
+      </c>
+      <c r="E5">
         <v>2</v>
       </c>
-      <c r="D5">
+      <c r="F5">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="C6">
+        <f>3.61*10^-6</f>
+        <v>3.6099999999999997E-6</v>
+      </c>
+      <c r="E6">
         <v>5</v>
       </c>
-      <c r="D6">
+      <c r="F6">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
       <c r="C7">
+        <f>67*10^-6</f>
+        <v>6.7000000000000002E-5</v>
+      </c>
+      <c r="E7">
         <v>2</v>
       </c>
-      <c r="D7">
+      <c r="F7">
         <v>1</v>
       </c>
-      <c r="E7">
+      <c r="G7">
         <v>3</v>
       </c>
-      <c r="F7">
+      <c r="H7">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
       <c r="C8">
+        <f>9.33*10^-6</f>
+        <v>9.3300000000000005E-6</v>
+      </c>
+      <c r="E8">
         <v>3</v>
       </c>
-      <c r="D8">
+      <c r="F8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
       <c r="C9">
+        <f>0.67*10^-6</f>
+        <v>6.7000000000000004E-7</v>
+      </c>
+      <c r="E9">
         <v>4</v>
       </c>
-      <c r="D9">
+      <c r="F9">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
       <c r="C10">
+        <f>67*10^-6</f>
+        <v>6.7000000000000002E-5</v>
+      </c>
+      <c r="E10">
         <v>2</v>
       </c>
-      <c r="D10">
+      <c r="F10">
         <v>3</v>
       </c>
-      <c r="E10">
+      <c r="G10">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
       <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="E11">
         <v>3</v>
       </c>
-      <c r="D11">
+      <c r="F11">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>17</v>
       </c>
       <c r="C12">
+        <f>0.67*10^-6</f>
+        <v>6.7000000000000004E-7</v>
+      </c>
+      <c r="E12">
         <v>4</v>
       </c>
-      <c r="D12">
+      <c r="F12">
         <v>3</v>
       </c>
     </row>
@@ -565,10 +613,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:A28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -576,145 +624,97 @@
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="str">
         <f>IF(Sheet1!A1="","",Sheet1!A1)</f>
         <v/>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>IF(Sheet1!A2="","",Sheet1!A2)</f>
         <v>Model</v>
       </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>IF(Sheet1!A3="","",Sheet1!A3)</f>
         <v>DSTWU</v>
       </c>
-      <c r="C3">
-        <f>67*10^-6</f>
-        <v>6.7000000000000002E-5</v>
-      </c>
-      <c r="D3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f>IF(Sheet1!A4="","",Sheet1!A4)</f>
         <v>MIXER</v>
       </c>
-      <c r="C4">
-        <f>6.7*10^-6</f>
-        <v>6.7000000000000002E-6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f>IF(Sheet1!A5="","",Sheet1!A5)</f>
         <v>SEP</v>
       </c>
-      <c r="C5">
-        <f>67*10^-6</f>
-        <v>6.7000000000000002E-5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f>IF(Sheet1!A6="","",Sheet1!A6)</f>
         <v>FSPLIT</v>
       </c>
-      <c r="C6">
-        <f>3.61*10^-6</f>
-        <v>3.6099999999999997E-6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f>IF(Sheet1!A7="","",Sheet1!A7)</f>
         <v>DISTL</v>
       </c>
-      <c r="C7">
-        <f>67*10^-6</f>
-        <v>6.7000000000000002E-5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f>IF(Sheet1!A8="","",Sheet1!A8)</f>
         <v>HEATER</v>
       </c>
-      <c r="C8">
-        <f>9.33*10^-6</f>
-        <v>9.3300000000000005E-6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f>IF(Sheet1!A9="","",Sheet1!A9)</f>
         <v>RGIBBS</v>
       </c>
-      <c r="C9">
-        <f>0.67*10^-6</f>
-        <v>6.7000000000000004E-7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f>IF(Sheet1!A10="","",Sheet1!A10)</f>
         <v>FLASH2</v>
       </c>
-      <c r="C10">
-        <f>67*10^-6</f>
-        <v>6.7000000000000002E-5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f>IF(Sheet1!A11="","",Sheet1!A11)</f>
         <v>COMPR</v>
       </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f>IF(Sheet1!A12="","",Sheet1!A12)</f>
         <v>RSTOIC</v>
       </c>
-      <c r="C12">
-        <f>0.67*10^-6</f>
-        <v>6.7000000000000004E-7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f>IF(Sheet1!A13="","",Sheet1!A13)</f>
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f>IF(Sheet1!A14="","",Sheet1!A14)</f>
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
         <f>IF(Sheet1!A15="","",Sheet1!A15)</f>
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f>IF(Sheet1!A16="","",Sheet1!A16)</f>
         <v/>

</xml_diff>